<commit_message>
updated python script for farfetch
</commit_message>
<xml_diff>
--- a/Updates/Input data/Bookings With Publisher Promo (10).xlsx
+++ b/Updates/Input data/Bookings With Publisher Promo (10).xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,48 +418,48 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>471191</v>
+        <v>476042</v>
       </c>
       <c r="B2" t="str">
-        <v>Vendor Assigned</v>
+        <v>Car Assigned</v>
       </c>
       <c r="C2" s="1">
-        <v>45943.12550925926</v>
+        <v>45956.12550925926</v>
       </c>
       <c r="D2" t="str">
-        <v>Monthly</v>
+        <v>Weekly</v>
       </c>
       <c r="E2" t="str">
         <v>Old</v>
       </c>
       <c r="F2">
-        <v>3543.73</v>
+        <v>1013.32</v>
       </c>
       <c r="G2">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>85.1352</v>
       </c>
       <c r="I2" t="str">
-        <v>D20</v>
+        <v>D95</v>
       </c>
       <c r="J2">
-        <v>0.0002</v>
+        <v>0.000325</v>
       </c>
       <c r="K2">
-        <v>70.87</v>
+        <v>32.93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>471974</v>
+        <v>477148</v>
       </c>
       <c r="B3" t="str">
-        <v>Rental Started</v>
+        <v>Car Assigned</v>
       </c>
       <c r="C3" s="1">
-        <v>45943.12550925926</v>
+        <v>45956.12550925926</v>
       </c>
       <c r="D3" t="str">
         <v>Daily</v>
@@ -468,13 +468,13 @@
         <v>Old</v>
       </c>
       <c r="F3">
-        <v>481.82</v>
+        <v>106.18</v>
       </c>
       <c r="G3">
         <v>0.1</v>
       </c>
       <c r="H3">
-        <v>53.535</v>
+        <v>11.798</v>
       </c>
       <c r="I3" t="str">
         <v>D95</v>
@@ -483,18 +483,18 @@
         <v>0.0003</v>
       </c>
       <c r="K3">
-        <v>14.45</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>472002</v>
+        <v>477159</v>
       </c>
       <c r="B4" t="str">
-        <v>Rental Started</v>
+        <v>Vendor Assigned</v>
       </c>
       <c r="C4" s="1">
-        <v>45943.12550925926</v>
+        <v>45956.12550925926</v>
       </c>
       <c r="D4" t="str">
         <v>Daily</v>
@@ -503,33 +503,33 @@
         <v>Old</v>
       </c>
       <c r="F4">
-        <v>89.98</v>
+        <v>101.67</v>
       </c>
       <c r="G4">
         <v>0.1</v>
       </c>
       <c r="H4">
-        <v>9.998</v>
+        <v>11.298</v>
       </c>
       <c r="I4" t="str">
-        <v>D95</v>
+        <v>D100</v>
       </c>
       <c r="J4">
         <v>0.0003</v>
       </c>
       <c r="K4">
-        <v>2.7</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>472251</v>
+        <v>477252</v>
       </c>
       <c r="B5" t="str">
         <v>Vendor Assigned</v>
       </c>
       <c r="C5" s="1">
-        <v>45943.12550925926</v>
+        <v>45956.12550925926</v>
       </c>
       <c r="D5" t="str">
         <v>Daily</v>
@@ -538,98 +538,28 @@
         <v>Old</v>
       </c>
       <c r="F5">
-        <v>565.15</v>
+        <v>690.9</v>
       </c>
       <c r="G5">
         <v>0.1</v>
       </c>
       <c r="H5">
-        <v>62.795</v>
+        <v>73.8924</v>
       </c>
       <c r="I5" t="str">
-        <v>Z99</v>
+        <v>D100</v>
       </c>
       <c r="J5">
         <v>0.0003</v>
       </c>
       <c r="K5">
-        <v>16.95</v>
+        <v>20.73</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6">
-        <v>472271</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Rental Started</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45943.12550925926</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Daily</v>
-      </c>
-      <c r="E6" t="str">
-        <v>New</v>
-      </c>
-      <c r="F6">
-        <v>321.94</v>
-      </c>
-      <c r="G6">
-        <v>0.1</v>
-      </c>
-      <c r="H6">
-        <v>34.293</v>
-      </c>
-      <c r="I6" t="str">
-        <v>D95</v>
-      </c>
-      <c r="J6">
-        <v>0.0003</v>
-      </c>
-      <c r="K6">
-        <v>9.66</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>472271</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Rental Started</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45943.12550925926</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Daily</v>
-      </c>
-      <c r="E7" t="str">
-        <v>New</v>
-      </c>
-      <c r="F7">
-        <v>-13.3</v>
-      </c>
-      <c r="G7">
-        <v>0.1</v>
-      </c>
-      <c r="H7">
-        <v>34.293</v>
-      </c>
-      <c r="I7" t="str">
-        <v>D95</v>
-      </c>
-      <c r="J7">
-        <v>0.0003</v>
-      </c>
-      <c r="K7">
-        <v>-0.4</v>
-      </c>
-    </row>
-    <row r="8"/>
+    <row r="6"/>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>